<commit_message>
added col for hani`s notes+ date for execution+ started with cutting the negative rows+  fixed the notes column
</commit_message>
<xml_diff>
--- a/gvia_month.xlsx
+++ b/gvia_month.xlsx
@@ -1227,9 +1227,9 @@
     <t>מייהריטאג' בעמ</t>
   </si>
   <si>
-    <t>03/07/2016 - חני :  ייעוץ חודשי -ה.בנקאית  (הנחה12%) ניהול חוזים - לשלוח לנעמי לוודא שקיבלה
-10/07/2016 - חני : התשלום אושר - אירנה תשלום בסוף החודש 31.7
-31/07/2016 - חני : שולם</t>
+    <t>10/07/2016 - חני : התשלום אושר - אירנה תשלום בסוף החודש 31.7
+31/07/2016 - חני : שולם
+10/08/2016 - חני : נשלחה לנעמי חן מס העתק שוב לאישור תשלום</t>
   </si>
   <si>
     <t>י. שפירא ושות' עורכי דין</t>

</xml_diff>